<commit_message>
Added correct folder structure for outputting excel files
</commit_message>
<xml_diff>
--- a/Templates/Payslip_template.xlsx
+++ b/Templates/Payslip_template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\22ruslanrakhmaninr\OneDrive - City of Dublin ETB\Procedural Programming (Python)\Group B\Payroll\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\25LukeMaycock\Desktop\Software Dev\Repos\PP\Payroll App\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{061A20C5-415A-4FCD-92DB-3C10A1A5F8F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="3090" yWindow="1215" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Payslip" sheetId="1" r:id="rId1"/>
@@ -19,6 +20,9 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -137,31 +141,31 @@
     <t>&lt;Hours&gt;</t>
   </si>
   <si>
-    <t>&lt;Rate&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Salary&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bonuses&gt;</t>
-  </si>
-  <si>
     <t>&lt;GrossPay&gt;</t>
   </si>
   <si>
-    <t>&lt;Taxes&gt;</t>
-  </si>
-  <si>
     <t>&lt;TotalDeductions&gt;</t>
   </si>
   <si>
     <t>&lt;NetPay&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Hourly Rate&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bonus&gt;</t>
+  </si>
+  <si>
+    <t>&lt;salary&gt;</t>
+  </si>
+  <si>
+    <t>&lt;tax&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
   </numFmts>
@@ -752,11 +756,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -897,10 +901,10 @@
         <v>36</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -910,7 +914,7 @@
       <c r="B14" s="27"/>
       <c r="C14" s="29"/>
       <c r="D14" s="28" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -946,7 +950,7 @@
         <v>20</v>
       </c>
       <c r="D18" s="33" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -972,7 +976,7 @@
       <c r="B21" s="27"/>
       <c r="C21" s="27"/>
       <c r="D21" s="28" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -994,7 +998,7 @@
         <v>23</v>
       </c>
       <c r="D24" s="33" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1010,7 +1014,7 @@
         <v>24</v>
       </c>
       <c r="D26" s="37" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1229,15 +1233,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="36d42694-3c0d-493d-b31b-c149c81705f0">
@@ -1248,14 +1243,49 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA23C947-DF4A-4345-A3C7-EFED5BE56085}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA23C947-DF4A-4345-A3C7-EFED5BE56085}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="36d42694-3c0d-493d-b31b-c149c81705f0"/>
+    <ds:schemaRef ds:uri="6d849b53-5f16-44bd-bccd-8b425bb601eb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1716E06B-6BCA-49E4-910C-E39E1361FB8F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{633850E6-3C1A-4099-9759-CB163B7B3D55}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="36d42694-3c0d-493d-b31b-c149c81705f0"/>
+    <ds:schemaRef ds:uri="6d849b53-5f16-44bd-bccd-8b425bb601eb"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{633850E6-3C1A-4099-9759-CB163B7B3D55}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1716E06B-6BCA-49E4-910C-E39E1361FB8F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add date generation to payslip and update design document with new requirement
</commit_message>
<xml_diff>
--- a/Templates/Payslip_template.xlsx
+++ b/Templates/Payslip_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\25LukeMaycock\Desktop\Software Dev\Repos\PP\Payroll App\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE194576-8770-409D-BA49-173F966517D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C50F106F-A25D-469A-8C2C-5D6FD04C1BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -374,7 +374,7 @@
     <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -409,9 +409,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -501,6 +498,12 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -787,7 +790,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -799,17 +802,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="35.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>28</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="20" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="3"/>
@@ -817,7 +820,7 @@
       <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="25" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="3"/>
@@ -831,14 +834,14 @@
       <c r="D4" s="7"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="21" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="6"/>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="23" t="s">
         <v>3</v>
       </c>
     </row>
@@ -847,10 +850,10 @@
         <v>21</v>
       </c>
       <c r="B6" s="6"/>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="38" t="s">
+      <c r="D6" s="37" t="s">
         <v>4</v>
       </c>
     </row>
@@ -862,7 +865,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="6"/>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="23" t="s">
         <v>22</v>
       </c>
     </row>
@@ -872,7 +875,7 @@
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
-      <c r="D8" s="39" t="s">
+      <c r="D8" s="38" t="s">
         <v>29</v>
       </c>
     </row>
@@ -889,175 +892,175 @@
         <v>6</v>
       </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="42" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="6"/>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="40" t="s">
+      <c r="C12" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="29" t="s">
+      <c r="D12" s="28" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="24" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="41" t="s">
+      <c r="C13" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="14" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="15" t="s">
+      <c r="B14" s="13"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="15"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="14"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="15"/>
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="14"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="15"/>
+      <c r="A17" s="13"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="14"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="32" t="s">
+      <c r="A18" s="29"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="33" t="s">
+      <c r="D18" s="32" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
+      <c r="A19" s="12"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
-      <c r="D19" s="17"/>
+      <c r="D19" s="16"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="29" t="s">
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="28" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="15" t="s">
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="14" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="15" t="s">
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="14" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="15"/>
+      <c r="A23" s="13"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="14"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="30"/>
-      <c r="B24" s="31"/>
-      <c r="C24" s="34" t="s">
+      <c r="A24" s="29"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="37">
+      <c r="D24" s="36">
         <f>SUM(D21:D23)</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="13"/>
+      <c r="A25" s="12"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
-      <c r="D25" s="17"/>
+      <c r="D25" s="16"/>
     </row>
     <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="13"/>
+      <c r="A26" s="12"/>
       <c r="B26" s="6"/>
-      <c r="C26" s="35" t="s">
+      <c r="C26" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="D26" s="36" t="s">
+      <c r="D26" s="35" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
+      <c r="A27" s="12"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="18" t="s">
+      <c r="A28" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="42" t="s">
+      <c r="A29" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Update output file format to include a CSV and enhance design document with bonus and benefit details
</commit_message>
<xml_diff>
--- a/Templates/Payslip_template.xlsx
+++ b/Templates/Payslip_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\25LukeMaycock\Desktop\Software Dev\Repos\PP\Payroll App\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C50F106F-A25D-469A-8C2C-5D6FD04C1BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC4B6EDF-FB61-4FD4-963B-846AD04AE1A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -424,86 +424,86 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="7" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="11" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="8" fontId="7" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="8" fontId="11" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -790,7 +790,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -802,17 +802,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="35.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="17" t="s">
         <v>28</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="18" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="3"/>
@@ -820,7 +820,7 @@
       <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="23" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="3"/>
@@ -834,14 +834,14 @@
       <c r="D4" s="7"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="6"/>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="21" t="s">
         <v>3</v>
       </c>
     </row>
@@ -850,10 +850,10 @@
         <v>21</v>
       </c>
       <c r="B6" s="6"/>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="37" t="s">
+      <c r="D6" s="35" t="s">
         <v>4</v>
       </c>
     </row>
@@ -865,7 +865,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="6"/>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="21" t="s">
         <v>22</v>
       </c>
     </row>
@@ -875,7 +875,7 @@
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
-      <c r="D8" s="38" t="s">
+      <c r="D8" s="36" t="s">
         <v>29</v>
       </c>
     </row>
@@ -892,10 +892,10 @@
         <v>6</v>
       </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="43" t="s">
+      <c r="C10" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="42" t="s">
+      <c r="D10" s="39" t="s">
         <v>32</v>
       </c>
     </row>
@@ -906,16 +906,16 @@
       <c r="D11" s="11"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="39" t="s">
+      <c r="C12" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="26" t="s">
         <v>11</v>
       </c>
     </row>
@@ -926,7 +926,7 @@
       <c r="B13" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="40" t="s">
+      <c r="C13" s="38" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="14" t="s">
@@ -944,10 +944,14 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
+      <c r="A15" s="13" t="s">
+        <v>30</v>
+      </c>
       <c r="B15" s="13"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="14"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
@@ -962,12 +966,12 @@
       <c r="D17" s="14"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="29"/>
-      <c r="B18" s="30"/>
-      <c r="C18" s="31" t="s">
+      <c r="A18" s="27"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="32" t="s">
+      <c r="D18" s="30" t="s">
         <v>35</v>
       </c>
     </row>
@@ -978,12 +982,12 @@
       <c r="D19" s="16"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="28" t="s">
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="26" t="s">
         <v>11</v>
       </c>
     </row>
@@ -995,16 +999,6 @@
       <c r="C21" s="13"/>
       <c r="D21" s="14" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="14" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1014,12 +1008,12 @@
       <c r="D23" s="14"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="29"/>
-      <c r="B24" s="30"/>
-      <c r="C24" s="33" t="s">
+      <c r="A24" s="27"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="36">
+      <c r="D24" s="34">
         <f>SUM(D21:D23)</f>
         <v>0</v>
       </c>
@@ -1033,10 +1027,10 @@
     <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="12"/>
       <c r="B26" s="6"/>
-      <c r="C26" s="34" t="s">
+      <c r="C26" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="D26" s="35" t="s">
+      <c r="D26" s="33" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1047,20 +1041,20 @@
       <c r="D27" s="6"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
+      <c r="B28" s="41"/>
+      <c r="C28" s="41"/>
+      <c r="D28" s="41"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="41" t="s">
+      <c r="A29" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="18"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1087,6 +1081,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010086DDA2978BE8B14CAB0F8A66BF4424BF" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fd997352884877366cea4e220f1165e4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="36d42694-3c0d-493d-b31b-c149c81705f0" xmlns:ns3="6d849b53-5f16-44bd-bccd-8b425bb601eb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4509ba76b6b53b90bf930da34c1a5827" ns2:_="" ns3:_="">
     <xsd:import namespace="36d42694-3c0d-493d-b31b-c149c81705f0"/>
@@ -1269,15 +1272,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{633850E6-3C1A-4099-9759-CB163B7B3D55}">
   <ds:schemaRefs>
@@ -1290,6 +1284,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1716E06B-6BCA-49E4-910C-E39E1361FB8F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA23C947-DF4A-4345-A3C7-EFED5BE56085}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1306,12 +1308,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1716E06B-6BCA-49E4-910C-E39E1361FB8F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Remove outdated design documents and templates from the repository
</commit_message>
<xml_diff>
--- a/Templates/Payslip_template.xlsx
+++ b/Templates/Payslip_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\25LukeMaycock\Desktop\Software Dev\Repos\PP\Payroll App\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC4B6EDF-FB61-4FD4-963B-846AD04AE1A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34A2184-764A-410D-9B43-EECC8C629A1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>PAYSLIP</t>
   </si>
@@ -57,9 +57,6 @@
     <t>[42]</t>
   </si>
   <si>
-    <t>Email: name@provider.com</t>
-  </si>
-  <si>
     <t>Payment Method:</t>
   </si>
   <si>
@@ -93,15 +90,6 @@
     <t>NET PAY</t>
   </si>
   <si>
-    <t>If you have any questions about this payslip, please contact:</t>
-  </si>
-  <si>
-    <t>Somewhere in Ireland</t>
-  </si>
-  <si>
-    <t>Phone: +353 00 0000 0000</t>
-  </si>
-  <si>
     <t>&lt;Name&gt;</t>
   </si>
   <si>
@@ -147,51 +135,36 @@
     <t>&lt;grosspay&gt;</t>
   </si>
   <si>
-    <t>Address 2</t>
-  </si>
-  <si>
-    <t>Address 1</t>
-  </si>
-  <si>
     <t>&lt;currentdate&gt;</t>
   </si>
   <si>
     <t>payroll@lmportraiture.com</t>
+  </si>
+  <si>
+    <t>Butterly Business Park, Artane, Dublin 5</t>
+  </si>
+  <si>
+    <t>Phone: +353 12 3456 7890</t>
+  </si>
+  <si>
+    <t>For payroll related queries please contact:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="24"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="24"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF28577D"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -226,11 +199,6 @@
     <font>
       <sz val="1"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -371,139 +339,128 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="8" fontId="7" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="8" fontId="11" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -787,10 +744,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="A7" sqref="A7:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -801,268 +758,276 @@
     <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="35.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="18" t="s">
+    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>3</v>
-      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="35" t="s">
-        <v>4</v>
-      </c>
+      <c r="A6" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="21" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="36" t="s">
-        <v>29</v>
-      </c>
+      <c r="A7" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="24" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="39" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="37" t="s">
+      <c r="D17" s="35" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="36"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="35" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="35" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="35"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C22" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="37" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="38"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="26" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="24" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="13" t="s">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="38" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="14"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="14"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="27"/>
-      <c r="B18" s="28"/>
-      <c r="C18" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="30" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="16"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="25"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="26" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D26" s="36"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="35"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C28" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="14"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
-      <c r="B24" s="28"/>
-      <c r="C24" s="31" t="s">
+      <c r="D28" s="19">
+        <f>SUM(D25:D27)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="6"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="38"/>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="6"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="34">
-        <f>SUM(D21:D23)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="12"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="16"/>
-    </row>
-    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="12"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="D26" s="33" t="s">
+      <c r="D30" s="40" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="23"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="23"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="24"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="30"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="31" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="B28" s="41"/>
-      <c r="C28" s="41"/>
-      <c r="D28" s="41"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="42" t="s">
-        <v>39</v>
-      </c>
-      <c r="B29" s="43"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="43"/>
+      <c r="B36" s="31"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="31"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A29:D29"/>
+  <mergeCells count="6">
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A7:D7"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A29" r:id="rId1" xr:uid="{A588EAA1-64E3-42BE-AE0B-B93A904C5A32}"/>
+    <hyperlink ref="A36" r:id="rId1" xr:uid="{A588EAA1-64E3-42BE-AE0B-B93A904C5A32}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="85" orientation="portrait" r:id="rId2"/>

</xml_diff>